<commit_message>
cater no such keyword
</commit_message>
<xml_diff>
--- a/Hybrid Keyword Driven/bin/dataEngine/DataEngine.xlsx
+++ b/Hybrid Keyword Driven/bin/dataEngine/DataEngine.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView windowHeight="2910" windowWidth="16500" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" windowHeight="2910" windowWidth="16500" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" r:id="rId1" sheetId="2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="80">
   <si>
     <t>Description</t>
   </si>
@@ -261,7 +261,13 @@
     <t>TS_7</t>
   </si>
   <si>
-    <t>PASS</t>
+    <t>Browser</t>
+  </si>
+  <si>
+    <t>eat</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
@@ -607,8 +613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,7 +650,7 @@
         <v>74</v>
       </c>
       <c r="D2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -679,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,13 +736,13 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>3</v>
+        <v>78</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="G2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -755,9 +761,6 @@
       <c r="E3" t="s">
         <v>7</v>
       </c>
-      <c r="G3" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -778,9 +781,6 @@
       <c r="F4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G4" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -801,9 +801,6 @@
       <c r="F5" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G5" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -822,9 +819,6 @@
         <v>7</v>
       </c>
       <c r="F6" s="7"/>
-      <c r="G6" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -845,9 +839,6 @@
       <c r="F7" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G7" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -864,9 +855,6 @@
         <v>12</v>
       </c>
       <c r="F8" s="7"/>
-      <c r="G8" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">

</xml_diff>

<commit_message>
commit to try git symbol in eclipse
</commit_message>
<xml_diff>
--- a/Hybrid Keyword Driven/bin/dataEngine/DataEngine.xlsx
+++ b/Hybrid Keyword Driven/bin/dataEngine/DataEngine.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="2910" windowWidth="16500" xWindow="0" yWindow="0"/>
+    <workbookView windowHeight="2910" windowWidth="16500" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" r:id="rId1" sheetId="2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="88">
   <si>
     <t>Description</t>
   </si>
@@ -240,31 +240,55 @@
     <t>//*[@id="page-container"]/div[2]/div/div[2]/div[1]</t>
   </si>
   <si>
-    <t>verify</t>
-  </si>
-  <si>
     <t>login</t>
   </si>
   <si>
-    <t>logout</t>
-  </si>
-  <si>
-    <t>verify username</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>TS_7</t>
-  </si>
-  <si>
     <t>Browser</t>
   </si>
   <si>
-    <t>eat</t>
+    <t>openbrowser</t>
+  </si>
+  <si>
+    <t>Chrome</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>//*[@id="page-container"]/div[2]/div/div[2]/div[2]/a</t>
+  </si>
+  <si>
+    <t>log keluar</t>
+  </si>
+  <si>
+    <t>click download button</t>
+  </si>
+  <si>
+    <t>//*[@id="page-container"]/div[5]/input[1]</t>
+  </si>
+  <si>
+    <t>verify android term</t>
+  </si>
+  <si>
+    <t>/html/body/div/div[1]/div[2]/div/div[1]/h3</t>
+  </si>
+  <si>
+    <t>android</t>
+  </si>
+  <si>
+    <t>verify ios term</t>
+  </si>
+  <si>
+    <t>/html/body/div/div[1]/div[3]/div/div[1]/h3</t>
+  </si>
+  <si>
+    <t>ios</t>
+  </si>
+  <si>
+    <t>PASS</t>
   </si>
   <si>
     <t>FAIL</t>
@@ -275,7 +299,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -294,6 +318,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -319,7 +350,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
@@ -331,6 +362,8 @@
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
     <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -611,10 +644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,38 +674,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
         <v>58</v>
       </c>
       <c r="C2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C4" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -683,10 +694,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -724,7 +735,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -736,18 +747,18 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="G2" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
@@ -761,10 +772,13 @@
       <c r="E3" t="s">
         <v>7</v>
       </c>
+      <c r="G3" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
@@ -781,10 +795,13 @@
       <c r="F4" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="G4" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
@@ -801,10 +818,13 @@
       <c r="F5" s="7" t="s">
         <v>26</v>
       </c>
+      <c r="G5" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B6" t="s">
         <v>22</v>
@@ -819,10 +839,13 @@
         <v>7</v>
       </c>
       <c r="F6" s="7"/>
+      <c r="G6" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B7" t="s">
         <v>23</v>
@@ -831,66 +854,80 @@
         <v>68</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="E7" t="s">
         <v>53</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>25</v>
+        <v>77</v>
+      </c>
+      <c r="G7" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B8" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="6"/>
+        <v>78</v>
+      </c>
+      <c r="D8" t="s">
+        <v>79</v>
+      </c>
       <c r="E8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="7"/>
+        <v>7</v>
+      </c>
+      <c r="F8"/>
+      <c r="G8" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>70</v>
       </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
-        <v>3</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>61</v>
+      <c r="B9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="G9" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>70</v>
       </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="E10" t="s">
-        <v>7</v>
+      <c r="B10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -898,92 +935,24 @@
         <v>70</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="E11" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>25</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>70</v>
-      </c>
-      <c r="B12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E12" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="D12" s="6"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>70</v>
-      </c>
-      <c r="B13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E13" t="s">
-        <v>7</v>
-      </c>
+      <c r="D13" s="6"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>70</v>
-      </c>
-      <c r="B14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" t="s">
-        <v>68</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="E14" t="s">
-        <v>53</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>70</v>
-      </c>
-      <c r="B15" t="s">
-        <v>76</v>
-      </c>
-      <c r="C15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="6"/>
-      <c r="E15" t="s">
-        <v>12</v>
-      </c>
+      <c r="D14" s="6"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -995,7 +964,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1022,7 +991,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>9</v>
@@ -1031,13 +1000,10 @@
         <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>71</v>
-      </c>
       <c r="B3" s="1" t="s">
         <v>41</v>
       </c>
@@ -1049,32 +1015,12 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" t="s">
-        <v>57</v>
-      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" t="s">
-        <v>57</v>
-      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
@@ -1462,7 +1408,7 @@
     </row>
     <row ht="45" r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B20" t="s">
         <v>23</v>

</xml_diff>